<commit_message>
update OSM_JRC_classification and change "tags"to "buildings" key
</commit_message>
<xml_diff>
--- a/hydromt_fiat/data/damage_functions/flooding/JRC_OSM_mapping.xlsx
+++ b/hydromt_fiat/data/damage_functions/flooding/JRC_OSM_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rautenba\repos\hydromt_fiat\hydromt_fiat\data\damage_functions\flooding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C311A424-16D3-43AD-B65A-31D2E317B6D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE0F884-6804-49E4-A6A6-6F679E537E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B17254A1-C85A-4773-BB08-3A5A1F2CE768}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B17254A1-C85A-4773-BB08-3A5A1F2CE768}"/>
   </bookViews>
   <sheets>
     <sheet name="landuse" sheetId="1" r:id="rId1"/>
@@ -23546,7 +23546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB02460E-BD7A-4088-9621-10DB89D5A4B0}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -23777,8 +23777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9442252E-E3A4-432E-9F36-0C4976D9D453}">
   <dimension ref="A1:B1923"/>
   <sheetViews>
-    <sheetView topLeftCell="A1383" workbookViewId="0">
-      <selection activeCell="E1406" sqref="E1406"/>
+    <sheetView topLeftCell="A1904" workbookViewId="0">
+      <selection activeCell="I1917" sqref="I1917"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23821,7 +23821,7 @@
         <v>1340</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -24325,7 +24325,7 @@
         <v>256</v>
       </c>
       <c r="B68" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -24341,7 +24341,7 @@
         <v>128</v>
       </c>
       <c r="B70" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -24349,7 +24349,7 @@
         <v>775</v>
       </c>
       <c r="B71" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -24357,7 +24357,7 @@
         <v>1867</v>
       </c>
       <c r="B72" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -24365,7 +24365,7 @@
         <v>1667</v>
       </c>
       <c r="B73" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -24389,7 +24389,7 @@
         <v>194</v>
       </c>
       <c r="B76" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -24405,7 +24405,7 @@
         <v>1620</v>
       </c>
       <c r="B78" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -24429,7 +24429,7 @@
         <v>1021</v>
       </c>
       <c r="B81" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -24437,7 +24437,7 @@
         <v>1262</v>
       </c>
       <c r="B82" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -24445,7 +24445,7 @@
         <v>1070</v>
       </c>
       <c r="B83" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -24461,7 +24461,7 @@
         <v>1680</v>
       </c>
       <c r="B85" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -24469,7 +24469,7 @@
         <v>571</v>
       </c>
       <c r="B86" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -24477,7 +24477,7 @@
         <v>707</v>
       </c>
       <c r="B87" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -24485,7 +24485,7 @@
         <v>137</v>
       </c>
       <c r="B88" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -24493,7 +24493,7 @@
         <v>167</v>
       </c>
       <c r="B89" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -24509,7 +24509,7 @@
         <v>716</v>
       </c>
       <c r="B91" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -25741,7 +25741,7 @@
         <v>700</v>
       </c>
       <c r="B245" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
@@ -25813,7 +25813,7 @@
         <v>829</v>
       </c>
       <c r="B254" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
@@ -25973,7 +25973,7 @@
         <v>79</v>
       </c>
       <c r="B274" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
@@ -26437,7 +26437,7 @@
         <v>210</v>
       </c>
       <c r="B332" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
@@ -26445,7 +26445,7 @@
         <v>1571</v>
       </c>
       <c r="B333" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
@@ -26461,7 +26461,7 @@
         <v>1234</v>
       </c>
       <c r="B335" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
@@ -26469,7 +26469,7 @@
         <v>1047</v>
       </c>
       <c r="B336" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
@@ -26517,7 +26517,7 @@
         <v>1519</v>
       </c>
       <c r="B342" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
@@ -26541,7 +26541,7 @@
         <v>370</v>
       </c>
       <c r="B345" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
@@ -26549,7 +26549,7 @@
         <v>411</v>
       </c>
       <c r="B346" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
@@ -27661,7 +27661,7 @@
         <v>1646</v>
       </c>
       <c r="B485" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="486" spans="1:2" x14ac:dyDescent="0.25">
@@ -28181,7 +28181,7 @@
         <v>1561</v>
       </c>
       <c r="B550" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="551" spans="1:2" x14ac:dyDescent="0.25">
@@ -28189,7 +28189,7 @@
         <v>1562</v>
       </c>
       <c r="B551" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="552" spans="1:2" x14ac:dyDescent="0.25">
@@ -28197,7 +28197,7 @@
         <v>1563</v>
       </c>
       <c r="B552" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="553" spans="1:2" x14ac:dyDescent="0.25">
@@ -28205,7 +28205,7 @@
         <v>1567</v>
       </c>
       <c r="B553" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="554" spans="1:2" x14ac:dyDescent="0.25">
@@ -28213,7 +28213,7 @@
         <v>1560</v>
       </c>
       <c r="B554" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="555" spans="1:2" x14ac:dyDescent="0.25">
@@ -32917,7 +32917,7 @@
         <v>203</v>
       </c>
       <c r="B1142" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1143" spans="1:2" x14ac:dyDescent="0.25">
@@ -32949,7 +32949,7 @@
         <v>838</v>
       </c>
       <c r="B1146" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1147" spans="1:2" x14ac:dyDescent="0.25">
@@ -32973,7 +32973,7 @@
         <v>681</v>
       </c>
       <c r="B1149" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1150" spans="1:2" x14ac:dyDescent="0.25">
@@ -32981,7 +32981,7 @@
         <v>211</v>
       </c>
       <c r="B1150" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1151" spans="1:2" x14ac:dyDescent="0.25">
@@ -33693,7 +33693,7 @@
         <v>1084</v>
       </c>
       <c r="B1239" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1240" spans="1:2" x14ac:dyDescent="0.25">
@@ -37037,7 +37037,7 @@
         <v>1251</v>
       </c>
       <c r="B1657" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1658" spans="1:2" x14ac:dyDescent="0.25">
@@ -37045,7 +37045,7 @@
         <v>1022</v>
       </c>
       <c r="B1658" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1659" spans="1:2" x14ac:dyDescent="0.25">
@@ -37053,7 +37053,7 @@
         <v>1418</v>
       </c>
       <c r="B1659" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1660" spans="1:2" x14ac:dyDescent="0.25">
@@ -37061,7 +37061,7 @@
         <v>1375</v>
       </c>
       <c r="B1660" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1661" spans="1:2" x14ac:dyDescent="0.25">
@@ -37869,7 +37869,7 @@
         <v>378</v>
       </c>
       <c r="B1761" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1762" spans="1:2" x14ac:dyDescent="0.25">
@@ -37877,7 +37877,7 @@
         <v>303</v>
       </c>
       <c r="B1762" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1763" spans="1:2" x14ac:dyDescent="0.25">
@@ -37885,7 +37885,7 @@
         <v>1057</v>
       </c>
       <c r="B1763" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1764" spans="1:2" x14ac:dyDescent="0.25">
@@ -38373,7 +38373,7 @@
         <v>1940</v>
       </c>
       <c r="B1824" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1825" spans="1:2" x14ac:dyDescent="0.25">
@@ -38381,7 +38381,7 @@
         <v>237</v>
       </c>
       <c r="B1825" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1826" spans="1:2" x14ac:dyDescent="0.25">
@@ -38389,7 +38389,7 @@
         <v>487</v>
       </c>
       <c r="B1826" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1827" spans="1:2" x14ac:dyDescent="0.25">
@@ -38397,7 +38397,7 @@
         <v>1829</v>
       </c>
       <c r="B1827" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1828" spans="1:2" x14ac:dyDescent="0.25">
@@ -38405,7 +38405,7 @@
         <v>1365</v>
       </c>
       <c r="B1828" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1829" spans="1:2" x14ac:dyDescent="0.25">
@@ -38413,7 +38413,7 @@
         <v>606</v>
       </c>
       <c r="B1829" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1830" spans="1:2" x14ac:dyDescent="0.25">
@@ -39069,7 +39069,7 @@
         <v>1065</v>
       </c>
       <c r="B1911" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1912" spans="1:2" x14ac:dyDescent="0.25">
@@ -39077,7 +39077,7 @@
         <v>250</v>
       </c>
       <c r="B1912" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1913" spans="1:2" x14ac:dyDescent="0.25">
@@ -39165,7 +39165,7 @@
         <v>844</v>
       </c>
       <c r="B1923" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -39180,8 +39180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28855F42-ACD8-491C-8FEB-8B394496C0E4}">
   <dimension ref="A1:B6129"/>
   <sheetViews>
-    <sheetView topLeftCell="A4088" workbookViewId="0">
-      <selection activeCell="D4115" sqref="D4115"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="T161" sqref="T161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41194,7 +41194,7 @@
         <v>41</v>
       </c>
       <c r="B251" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
@@ -41626,7 +41626,7 @@
         <v>2143</v>
       </c>
       <c r="B305" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
@@ -44002,7 +44002,7 @@
         <v>128</v>
       </c>
       <c r="B602" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.25">
@@ -44018,7 +44018,7 @@
         <v>606</v>
       </c>
       <c r="B604" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="605" spans="1:2" x14ac:dyDescent="0.25">
@@ -55882,7 +55882,7 @@
         <v>210</v>
       </c>
       <c r="B2087" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2088" spans="1:2" x14ac:dyDescent="0.25">
@@ -59794,7 +59794,7 @@
         <v>775</v>
       </c>
       <c r="B2576" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2577" spans="1:2" x14ac:dyDescent="0.25">
@@ -62362,7 +62362,7 @@
         <v>4495</v>
       </c>
       <c r="B2897" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2898" spans="1:2" x14ac:dyDescent="0.25">
@@ -70530,7 +70530,7 @@
         <v>5505</v>
       </c>
       <c r="B3918" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3919" spans="1:2" x14ac:dyDescent="0.25">
@@ -75186,7 +75186,7 @@
         <v>6087</v>
       </c>
       <c r="B4500" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4501" spans="1:2" x14ac:dyDescent="0.25">
@@ -77602,7 +77602,7 @@
         <v>6385</v>
       </c>
       <c r="B4802" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4803" spans="1:2" x14ac:dyDescent="0.25">
@@ -77802,7 +77802,7 @@
         <v>6410</v>
       </c>
       <c r="B4827" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4828" spans="1:2" x14ac:dyDescent="0.25">
@@ -78234,7 +78234,7 @@
         <v>838</v>
       </c>
       <c r="B4881" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4882" spans="1:2" x14ac:dyDescent="0.25">
@@ -82802,7 +82802,7 @@
         <v>7033</v>
       </c>
       <c r="B5452" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5453" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add header to excel sheet
</commit_message>
<xml_diff>
--- a/hydromt_fiat/data/damage_functions/flooding/JRC_OSM_mapping.xlsx
+++ b/hydromt_fiat/data/damage_functions/flooding/JRC_OSM_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rautenba\repos\hydromt_fiat\hydromt_fiat\data\damage_functions\flooding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE0F884-6804-49E4-A6A6-6F679E537E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11252991-99FC-4FE4-B831-499D4EDCA79B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B17254A1-C85A-4773-BB08-3A5A1F2CE768}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16149" uniqueCount="7705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16150" uniqueCount="7705">
   <si>
     <t>commercial</t>
   </si>
@@ -23159,7 +23159,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23171,14 +23171,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -23201,17 +23193,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -23546,7 +23535,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB02460E-BD7A-4088-9621-10DB89D5A4B0}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -23777,8 +23768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9442252E-E3A4-432E-9F36-0C4976D9D453}">
   <dimension ref="A1:B1923"/>
   <sheetViews>
-    <sheetView topLeftCell="A1904" workbookViewId="0">
-      <selection activeCell="I1917" sqref="I1917"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23790,7 +23781,9 @@
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -39180,8 +39173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28855F42-ACD8-491C-8FEB-8B394496C0E4}">
   <dimension ref="A1:B6129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="T161" sqref="T161"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C159" sqref="C1:C159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>